<commit_message>
added post-filter attenuator network
</commit_message>
<xml_diff>
--- a/power and current.xlsx
+++ b/power and current.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/git.nosync/aes17_filter_25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B678F93-6442-D141-A7AA-9B1D0D13CAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA88885E-6AE6-B343-8A77-60E0CE6375AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{350DCFA2-C205-4244-9A4F-11655FF7198F}"/>
+    <workbookView xWindow="1680" yWindow="7460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{350DCFA2-C205-4244-9A4F-11655FF7198F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>R1</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>R11</t>
+  </si>
+  <si>
+    <t>Wrms for each Vrms in divider network</t>
   </si>
 </sst>
 </file>
@@ -116,7 +120,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -179,11 +183,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -199,11 +223,81 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -539,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF99BDC2-D608-9743-AF0E-00E8EF7ED811}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,35 +685,35 @@
         <v>500</v>
       </c>
       <c r="C3" s="1">
-        <f>(($B3/$B$9)*C$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*C$2)^2/($B3*2)</f>
         <v>7.1769777253022674E-4</v>
       </c>
       <c r="D3" s="1">
-        <f>(($B3/$B$9)*D$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*D$2)^2/($B3*2)</f>
         <v>1.1483164360483628E-2</v>
       </c>
       <c r="E3" s="1">
-        <f>(($B3/$B$9)*E$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*E$2)^2/($B3*2)</f>
         <v>7.1769777253022665E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>(($B3/$B$9)*F$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*F$2)^2/($B3*2)</f>
         <v>0.28707910901209066</v>
       </c>
       <c r="G3" s="1">
-        <f>(($B3/$B$9)*G$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*G$2)^2/($B3*2)</f>
         <v>1.1483164360483626</v>
       </c>
       <c r="H3" s="1">
-        <f>(($B3/$B$9)*H$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*H$2)^2/($B3*2)</f>
         <v>2.5837119811088161</v>
       </c>
       <c r="I3" s="1">
-        <f>(($B3/$B$9)*I$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*I$2)^2/($B3*2)</f>
         <v>4.0370499704825251</v>
       </c>
       <c r="J3" s="1">
-        <f>(($B3/$B$9)*J$2)^2/($B3*2)</f>
+        <f>(($B3/$B$8)*J$2)^2/($B3*2)</f>
         <v>14.066876341592444</v>
       </c>
     </row>
@@ -631,35 +725,35 @@
         <v>0.1</v>
       </c>
       <c r="C4" s="1">
-        <f>(($B4/$B$9)*C$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*C$2)^2/($B4*2)</f>
         <v>1.4353955450604533E-7</v>
       </c>
       <c r="D4" s="1">
-        <f>(($B4/$B$9)*D$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*D$2)^2/($B4*2)</f>
         <v>2.2966328720967252E-6</v>
       </c>
       <c r="E4" s="1">
-        <f>(($B4/$B$9)*E$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*E$2)^2/($B4*2)</f>
         <v>1.4353955450604532E-5</v>
       </c>
       <c r="F4" s="1">
-        <f>(($B4/$B$9)*F$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*F$2)^2/($B4*2)</f>
         <v>5.7415821802418127E-5</v>
       </c>
       <c r="G4" s="1">
-        <f>(($B4/$B$9)*G$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*G$2)^2/($B4*2)</f>
         <v>2.2966328720967251E-4</v>
       </c>
       <c r="H4" s="1">
-        <f>(($B4/$B$9)*H$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*H$2)^2/($B4*2)</f>
         <v>5.1674239622176324E-4</v>
       </c>
       <c r="I4" s="1">
-        <f>(($B4/$B$9)*I$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*I$2)^2/($B4*2)</f>
         <v>8.0740999409650513E-4</v>
       </c>
       <c r="J4" s="1">
-        <f>(($B4/$B$9)*J$2)^2/($B4*2)</f>
+        <f>(($B4/$B$8)*J$2)^2/($B4*2)</f>
         <v>2.813375268318488E-3</v>
       </c>
     </row>
@@ -671,35 +765,35 @@
         <v>68</v>
       </c>
       <c r="C5" s="1">
-        <f>(($B5/$B$9)*C$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*C$2)^2/($B5*2)</f>
         <v>9.7606897064110847E-5</v>
       </c>
       <c r="D5" s="1">
-        <f>(($B5/$B$9)*D$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*D$2)^2/($B5*2)</f>
         <v>1.5617103530257736E-3</v>
       </c>
       <c r="E5" s="1">
-        <f>(($B5/$B$9)*E$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*E$2)^2/($B5*2)</f>
         <v>9.7606897064110819E-3</v>
       </c>
       <c r="F5" s="1">
-        <f>(($B5/$B$9)*F$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*F$2)^2/($B5*2)</f>
         <v>3.9042758825644328E-2</v>
       </c>
       <c r="G5" s="1">
-        <f>(($B5/$B$9)*G$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*G$2)^2/($B5*2)</f>
         <v>0.15617103530257731</v>
       </c>
       <c r="H5" s="1">
-        <f>(($B5/$B$9)*H$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*H$2)^2/($B5*2)</f>
         <v>0.35138482943079907</v>
       </c>
       <c r="I5" s="1">
-        <f>(($B5/$B$9)*I$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*I$2)^2/($B5*2)</f>
         <v>0.54903879598562355</v>
       </c>
       <c r="J5" s="1">
-        <f>(($B5/$B$9)*J$2)^2/($B5*2)</f>
+        <f>(($B5/$B$8)*J$2)^2/($B5*2)</f>
         <v>1.9130951824565723</v>
       </c>
     </row>
@@ -711,35 +805,35 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="1">
-        <f>(($B6/$B$9)*C$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*C$2)^2/($B6*2)</f>
         <v>1.4353955450604533E-7</v>
       </c>
       <c r="D6" s="1">
-        <f>(($B6/$B$9)*D$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*D$2)^2/($B6*2)</f>
         <v>2.2966328720967252E-6</v>
       </c>
       <c r="E6" s="1">
-        <f>(($B6/$B$9)*E$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*E$2)^2/($B6*2)</f>
         <v>1.4353955450604532E-5</v>
       </c>
       <c r="F6" s="1">
-        <f>(($B6/$B$9)*F$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*F$2)^2/($B6*2)</f>
         <v>5.7415821802418127E-5</v>
       </c>
       <c r="G6" s="1">
-        <f>(($B6/$B$9)*G$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*G$2)^2/($B6*2)</f>
         <v>2.2966328720967251E-4</v>
       </c>
       <c r="H6" s="1">
-        <f>(($B6/$B$9)*H$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*H$2)^2/($B6*2)</f>
         <v>5.1674239622176324E-4</v>
       </c>
       <c r="I6" s="1">
-        <f>(($B6/$B$9)*I$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*I$2)^2/($B6*2)</f>
         <v>8.0740999409650513E-4</v>
       </c>
       <c r="J6" s="1">
-        <f>(($B6/$B$9)*J$2)^2/($B6*2)</f>
+        <f>(($B6/$B$8)*J$2)^2/($B6*2)</f>
         <v>2.813375268318488E-3</v>
       </c>
     </row>
@@ -751,36 +845,559 @@
         <v>22</v>
       </c>
       <c r="C7" s="1">
+        <f>(($B7/$B$8)*C$2)^2/($B7*2)</f>
+        <v>3.1578701991329969E-5</v>
+      </c>
+      <c r="D7" s="1">
+        <f>(($B7/$B$8)*D$2)^2/($B7*2)</f>
+        <v>5.0525923186127951E-4</v>
+      </c>
+      <c r="E7" s="1">
+        <f>(($B7/$B$8)*E$2)^2/($B7*2)</f>
+        <v>3.1578701991329975E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <f>(($B7/$B$8)*F$2)^2/($B7*2)</f>
+        <v>1.263148079653199E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(($B7/$B$8)*G$2)^2/($B7*2)</f>
+        <v>5.0525923186127961E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <f>(($B7/$B$8)*H$2)^2/($B7*2)</f>
+        <v>0.1136833271687879</v>
+      </c>
+      <c r="I7" s="1">
+        <f>(($B7/$B$8)*I$2)^2/($B7*2)</f>
+        <v>0.17763019870123109</v>
+      </c>
+      <c r="J7" s="1">
+        <f>(($B7/$B$8)*J$2)^2/($B7*2)</f>
+        <v>0.61894255903006745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUM(B3:B7)</f>
+        <v>590.20000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2">
+        <v>40</v>
+      </c>
+      <c r="H10" s="2">
+        <v>60</v>
+      </c>
+      <c r="I10" s="2">
+        <v>75</v>
+      </c>
+      <c r="J10" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:J11" si="0">(C$10/$B$8)/2</f>
+        <v>8.4717045069467966E-4</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3886818027787187E-3</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>8.4717045069467971E-3</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6943409013893594E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3886818027787188E-2</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0830227041680782E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3537783802100983E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11860386309725515</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2">
+        <v>60</v>
+      </c>
+      <c r="I15" s="2">
+        <v>75</v>
+      </c>
+      <c r="J15" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>680</v>
+      </c>
+      <c r="C16" s="1">
+        <f>((C$15*$B16/$B$19)^2)/$B16/2</f>
+        <v>3.4000000000000008E-4</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D16:J16" si="1">((D$15*$B16/$B$19)^2)/$B16/2</f>
+        <v>5.4400000000000013E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3999999999999996E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13599999999999998</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.54399999999999993</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.224</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6640000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>220</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" ref="C17:J18" si="2">((C$15*$B17/$B$19)^2)/$B17/2</f>
+        <v>1.0999999999999999E-4</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7599999999999998E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17600000000000002</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.39599999999999996</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.61875000000000002</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1560000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000009E-5</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>8.0000000000000015E-4</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.18</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.28125</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <f>SUM(B16:B18)</f>
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C9:J9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:J7 C11:J11">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="greaterThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:J18">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DCD77F-8AAE-E84F-AB92-04AB9C1496F2}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2">
+        <v>60</v>
+      </c>
+      <c r="I2" s="2">
+        <v>75</v>
+      </c>
+      <c r="J2" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3" s="1">
+        <f>(($B3/$B$9)*C$2)^2/($B3*2)</f>
+        <v>2.7182204785954612E-6</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(($B3/$B$9)*D$2)^2/($B3*2)</f>
+        <v>4.349152765752738E-5</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(($B3/$B$9)*E$2)^2/($B3*2)</f>
+        <v>2.7182204785954615E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(($B3/$B$9)*F$2)^2/($B3*2)</f>
+        <v>1.0872881914381846E-3</v>
+      </c>
+      <c r="G3" s="1">
+        <f>(($B3/$B$9)*G$2)^2/($B3*2)</f>
+        <v>4.3491527657527384E-3</v>
+      </c>
+      <c r="H3" s="1">
+        <f>(($B3/$B$9)*H$2)^2/($B3*2)</f>
+        <v>9.7855937229436585E-3</v>
+      </c>
+      <c r="I3" s="1">
+        <f>(($B3/$B$9)*I$2)^2/($B3*2)</f>
+        <v>1.5289990192099472E-2</v>
+      </c>
+      <c r="J3" s="1">
+        <f>(($B3/$B$9)*J$2)^2/($B3*2)</f>
+        <v>5.3277121380471047E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="1">
+        <f>(($B4/$B$9)*C$2)^2/($B4*2)</f>
+        <v>5.4364409571909224E-10</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(($B4/$B$9)*D$2)^2/($B4*2)</f>
+        <v>8.6983055315054758E-9</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(($B4/$B$9)*E$2)^2/($B4*2)</f>
+        <v>5.4364409571909219E-8</v>
+      </c>
+      <c r="F4" s="1">
+        <f>(($B4/$B$9)*F$2)^2/($B4*2)</f>
+        <v>2.1745763828763688E-7</v>
+      </c>
+      <c r="G4" s="1">
+        <f>(($B4/$B$9)*G$2)^2/($B4*2)</f>
+        <v>8.698305531505475E-7</v>
+      </c>
+      <c r="H4" s="1">
+        <f>(($B4/$B$9)*H$2)^2/($B4*2)</f>
+        <v>1.957118744588732E-6</v>
+      </c>
+      <c r="I4" s="1">
+        <f>(($B4/$B$9)*I$2)^2/($B4*2)</f>
+        <v>3.0579980384198942E-6</v>
+      </c>
+      <c r="J4" s="1">
+        <f>(($B4/$B$9)*J$2)^2/($B4*2)</f>
+        <v>1.065542427609421E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1">
+        <f>(($B5/$B$9)*C$2)^2/($B5*2)</f>
+        <v>3.6967798508898273E-7</v>
+      </c>
+      <c r="D5" s="1">
+        <f>(($B5/$B$9)*D$2)^2/($B5*2)</f>
+        <v>5.9148477614237236E-6</v>
+      </c>
+      <c r="E5" s="1">
+        <f>(($B5/$B$9)*E$2)^2/($B5*2)</f>
+        <v>3.6967798508898279E-5</v>
+      </c>
+      <c r="F5" s="1">
+        <f>(($B5/$B$9)*F$2)^2/($B5*2)</f>
+        <v>1.4787119403559312E-4</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(($B5/$B$9)*G$2)^2/($B5*2)</f>
+        <v>5.9148477614237246E-4</v>
+      </c>
+      <c r="H5" s="1">
+        <f>(($B5/$B$9)*H$2)^2/($B5*2)</f>
+        <v>1.3308407463203376E-3</v>
+      </c>
+      <c r="I5" s="1">
+        <f>(($B5/$B$9)*I$2)^2/($B5*2)</f>
+        <v>2.0794386661255283E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <f>(($B5/$B$9)*J$2)^2/($B5*2)</f>
+        <v>7.2456885077440613E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="1">
+        <f>(($B6/$B$9)*C$2)^2/($B6*2)</f>
+        <v>5.4364409571909224E-10</v>
+      </c>
+      <c r="D6" s="1">
+        <f>(($B6/$B$9)*D$2)^2/($B6*2)</f>
+        <v>8.6983055315054758E-9</v>
+      </c>
+      <c r="E6" s="1">
+        <f>(($B6/$B$9)*E$2)^2/($B6*2)</f>
+        <v>5.4364409571909219E-8</v>
+      </c>
+      <c r="F6" s="1">
+        <f>(($B6/$B$9)*F$2)^2/($B6*2)</f>
+        <v>2.1745763828763688E-7</v>
+      </c>
+      <c r="G6" s="1">
+        <f>(($B6/$B$9)*G$2)^2/($B6*2)</f>
+        <v>8.698305531505475E-7</v>
+      </c>
+      <c r="H6" s="1">
+        <f>(($B6/$B$9)*H$2)^2/($B6*2)</f>
+        <v>1.957118744588732E-6</v>
+      </c>
+      <c r="I6" s="1">
+        <f>(($B6/$B$9)*I$2)^2/($B6*2)</f>
+        <v>3.0579980384198942E-6</v>
+      </c>
+      <c r="J6" s="1">
+        <f>(($B6/$B$9)*J$2)^2/($B6*2)</f>
+        <v>1.065542427609421E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
         <f>(($B7/$B$9)*C$2)^2/($B7*2)</f>
-        <v>3.1578701991329969E-5</v>
+        <v>1.1960170105820031E-7</v>
       </c>
       <c r="D7" s="1">
         <f>(($B7/$B$9)*D$2)^2/($B7*2)</f>
-        <v>5.0525923186127951E-4</v>
+        <v>1.913627216931205E-6</v>
       </c>
       <c r="E7" s="1">
         <f>(($B7/$B$9)*E$2)^2/($B7*2)</f>
-        <v>3.1578701991329975E-3</v>
+        <v>1.1960170105820032E-5</v>
       </c>
       <c r="F7" s="1">
         <f>(($B7/$B$9)*F$2)^2/($B7*2)</f>
-        <v>1.263148079653199E-2</v>
+        <v>4.7840680423280127E-5</v>
       </c>
       <c r="G7" s="1">
         <f>(($B7/$B$9)*G$2)^2/($B7*2)</f>
-        <v>5.0525923186127961E-2</v>
+        <v>1.9136272169312051E-4</v>
       </c>
       <c r="H7" s="1">
         <f>(($B7/$B$9)*H$2)^2/($B7*2)</f>
-        <v>0.1136833271687879</v>
+        <v>4.3056612380952108E-4</v>
       </c>
       <c r="I7" s="1">
         <f>(($B7/$B$9)*I$2)^2/($B7*2)</f>
-        <v>0.17763019870123109</v>
+        <v>6.7275956845237685E-4</v>
       </c>
       <c r="J7" s="1">
         <f>(($B7/$B$9)*J$2)^2/($B7*2)</f>
-        <v>0.61894255903006745</v>
+        <v>2.3441933407407265E-3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -788,39 +1405,39 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4500</v>
+        <v>9000</v>
       </c>
       <c r="C8" s="1">
-        <f>(C2*0.9)^2/$B8</f>
-        <v>1.8000000000000001E-4</v>
+        <f>(($B8/$B$9)*C$2)^2/($B8*2)</f>
+        <v>4.8927968614718301E-5</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:J8" si="0">(D2*0.9)^2/$B8</f>
-        <v>2.8800000000000002E-3</v>
+        <f>(($B8/$B$9)*D$2)^2/($B8*2)</f>
+        <v>7.8284749783549281E-4</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999999E-2</v>
+        <f>(($B8/$B$9)*E$2)^2/($B8*2)</f>
+        <v>4.8927968614718292E-3</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>7.1999999999999995E-2</v>
+        <f>(($B8/$B$9)*F$2)^2/($B8*2)</f>
+        <v>1.9571187445887317E-2</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.28799999999999998</v>
+        <f>(($B8/$B$9)*G$2)^2/($B8*2)</f>
+        <v>7.8284749783549268E-2</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.64800000000000002</v>
+        <f>(($B8/$B$9)*H$2)^2/($B8*2)</f>
+        <v>0.17614068701298588</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0125</v>
+        <f>(($B8/$B$9)*I$2)^2/($B8*2)</f>
+        <v>0.27521982345779045</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="0"/>
-        <v>3.528</v>
+        <f>(($B8/$B$9)*J$2)^2/($B8*2)</f>
+        <v>0.9589881848484787</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -828,8 +1445,8 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <f>SUM(B3:B7)</f>
-        <v>590.20000000000005</v>
+        <f>SUM(B3:B8)</f>
+        <v>9590.2000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -872,84 +1489,206 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="1">
-        <f>(C$11/$B$9)/2</f>
-        <v>8.4717045069467966E-4</v>
+        <f t="shared" ref="C12:J12" si="0">(C$11/$B$9)/2</f>
+        <v>5.2136556067652391E-5</v>
       </c>
       <c r="D12" s="1">
-        <f>(D$11/$B$9)/2</f>
-        <v>3.3886818027787187E-3</v>
+        <f t="shared" si="0"/>
+        <v>2.0854622427060956E-4</v>
       </c>
       <c r="E12" s="1">
-        <f>(E$11/$B$9)/2</f>
-        <v>8.4717045069467971E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.2136556067652396E-4</v>
       </c>
       <c r="F12" s="1">
-        <f>(F$11/$B$9)/2</f>
-        <v>1.6943409013893594E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.0427311213530479E-3</v>
       </c>
       <c r="G12" s="1">
-        <f>(G$11/$B$9)/2</f>
-        <v>3.3886818027787188E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.0854622427060958E-3</v>
       </c>
       <c r="H12" s="1">
-        <f>(H$11/$B$9)/2</f>
-        <v>5.0830227041680782E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.1281933640591435E-3</v>
       </c>
       <c r="I12" s="1">
-        <f>(I$11/$B$9)/2</f>
-        <v>6.3537783802100983E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.910241705073929E-3</v>
       </c>
       <c r="J12" s="1">
-        <f>(J$11/$B$9)/2</f>
-        <v>0.11860386309725515</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>7.2991178494713344E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <v>20</v>
+      </c>
+      <c r="G16" s="2">
+        <v>40</v>
+      </c>
+      <c r="H16" s="2">
+        <v>60</v>
+      </c>
+      <c r="I16" s="2">
+        <v>75</v>
+      </c>
+      <c r="J16" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>680</v>
+      </c>
+      <c r="C17" s="1">
+        <f>((C$16*$B17/$B$20)^2)/$B17/2</f>
+        <v>3.4000000000000008E-4</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" ref="D17:J17" si="1">((D$16*$B17/$B$20)^2)/$B17/2</f>
+        <v>5.4400000000000013E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3999999999999996E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13599999999999998</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.54399999999999993</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.224</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9125000000000001</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6640000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>220</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:J19" si="2">((C$16*$B18/$B$20)^2)/$B18/2</f>
+        <v>1.0999999999999999E-4</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7599999999999998E-3</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.17600000000000002</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.39599999999999996</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.61875000000000002</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1560000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000009E-5</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>8.0000000000000015E-4</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.18</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.28125</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2">
+        <f>SUM(B17:B19)</f>
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C15:J15"/>
   </mergeCells>
-  <conditionalFormatting sqref="C16:J19 C12:J12 C3:J8">
+  <conditionalFormatting sqref="C3:J8 C12:J12">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
@@ -960,6 +1699,18 @@
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C17:J19">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>